<commit_message>
group filtering functinality for missingness, incl. example
modified test data to produce some output for missingness
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jak2043/work/git/MT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3C8349-12F7-EF4A-A82A-DCF5D48EBA66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A7678-82A2-F144-93E5-0821D47D2ADB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrigScale" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -3056,8 +3056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="I14" workbookViewId="0">
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4418,18 +4418,10 @@
       <c r="R21" s="9">
         <v>34099</v>
       </c>
-      <c r="S21" s="9">
-        <v>77294</v>
-      </c>
-      <c r="T21" s="9">
-        <v>46569</v>
-      </c>
-      <c r="U21" s="9">
-        <v>30652</v>
-      </c>
-      <c r="V21" s="9">
-        <v>19312</v>
-      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
       <c r="W21" s="9">
         <v>42981</v>
       </c>
@@ -5180,18 +5172,10 @@
       <c r="V31" s="9">
         <v>42717</v>
       </c>
-      <c r="W31" s="9">
-        <v>31121</v>
-      </c>
-      <c r="X31" s="9">
-        <v>31724</v>
-      </c>
-      <c r="Y31" s="9">
-        <v>34413</v>
-      </c>
-      <c r="Z31" s="9">
-        <v>50705</v>
-      </c>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -6083,15 +6067,9 @@
       <c r="S44" s="9">
         <v>191620</v>
       </c>
-      <c r="T44" s="9">
-        <v>195591</v>
-      </c>
-      <c r="U44" s="9">
-        <v>104425</v>
-      </c>
-      <c r="V44" s="9">
-        <v>191652</v>
-      </c>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
       <c r="W44" s="9">
         <v>134987</v>
       </c>

</xml_diff>

<commit_message>
Removed double annotation for KEGG identifiers
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jak2043/work/git/MT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elb4003/Work/GitLab/krumsieklab/mt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A7678-82A2-F144-93E5-0821D47D2ADB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016C4C8C-05EC-CF46-BFF7-78C634F73542}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2448,9 +2448,6 @@
     <t>58-97-9</t>
   </si>
   <si>
-    <t>C01368, C00105</t>
-  </si>
-  <si>
     <t>HMDB00288</t>
   </si>
   <si>
@@ -2614,6 +2611,9 @@
   </si>
   <si>
     <t>treatment2</t>
+  </si>
+  <si>
+    <t>C01368</t>
   </si>
 </sst>
 </file>
@@ -3056,8 +3056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I14" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="H222" workbookViewId="0">
+      <selection activeCell="M227" sqref="M227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3132,7 +3132,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="O2" s="5">
         <v>69</v>
@@ -3188,40 +3188,40 @@
         <v>1</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="S3" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="Y3" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="Z3" s="5" t="s">
         <v>861</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -3238,43 +3238,43 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="Q4" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="S4" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="T4" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="U4" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="V4" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="W4" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="X4" s="5" t="s">
         <v>849</v>
       </c>
-      <c r="X4" s="5" t="s">
-        <v>850</v>
-      </c>
       <c r="Y4" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="Z4" s="5" t="s">
         <v>849</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -3291,7 +3291,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="O5" s="5">
         <v>1</v>
@@ -3344,7 +3344,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="O6" s="5">
         <v>1</v>
@@ -3397,43 +3397,43 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="P7" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="P7" s="5" t="s">
-        <v>856</v>
-      </c>
       <c r="Q7" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="T7" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="W7" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="X7" s="5" t="s">
         <v>855</v>
       </c>
-      <c r="V7" s="5" t="s">
-        <v>855</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>856</v>
-      </c>
-      <c r="X7" s="5" t="s">
-        <v>856</v>
-      </c>
       <c r="Y7" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -3450,43 +3450,43 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="P8" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="Q8" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="Q8" s="5" t="s">
-        <v>860</v>
-      </c>
       <c r="R8" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="S8" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="T8" s="5" t="s">
-        <v>860</v>
-      </c>
       <c r="U8" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="W8" s="5" t="s">
-        <v>860</v>
-      </c>
       <c r="X8" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="Y8" s="5" t="s">
         <v>858</v>
       </c>
-      <c r="Y8" s="5" t="s">
+      <c r="Z8" s="5" t="s">
         <v>859</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="48" x14ac:dyDescent="0.2">
@@ -3533,40 +3533,40 @@
         <v>15</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="S9" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="W9" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="T9" s="5" t="s">
+      <c r="X9" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="Y9" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="Z9" s="5" t="s">
         <v>861</v>
-      </c>
-      <c r="W9" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="Y9" s="5" t="s">
-        <v>862</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -19883,10 +19883,10 @@
       </c>
       <c r="L227" s="1"/>
       <c r="M227" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="N227" s="6" t="s">
         <v>807</v>
-      </c>
-      <c r="N227" s="6" t="s">
-        <v>808</v>
       </c>
       <c r="O227" s="9">
         <v>364170</v>
@@ -19930,7 +19930,7 @@
         <v>258</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>85</v>
@@ -19954,7 +19954,7 @@
         <v>118.1</v>
       </c>
       <c r="J228" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="K228" s="1">
         <v>6287</v>
@@ -19963,10 +19963,10 @@
         <v>6050</v>
       </c>
       <c r="M228" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="N228" s="6" t="s">
         <v>811</v>
-      </c>
-      <c r="N228" s="6" t="s">
-        <v>812</v>
       </c>
       <c r="O228" s="9">
         <v>1744768</v>
@@ -20010,7 +20010,7 @@
         <v>678</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>142</v>
@@ -20034,7 +20034,7 @@
         <v>173.1</v>
       </c>
       <c r="J229" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="K229" s="1">
         <v>136487</v>
@@ -20062,7 +20062,7 @@
         <v>680</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>142</v>
@@ -20086,10 +20086,10 @@
         <v>231.2</v>
       </c>
       <c r="J230" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="K230" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="K230" s="1" t="s">
-        <v>817</v>
       </c>
       <c r="L230" s="1">
         <v>4414314</v>
@@ -20114,7 +20114,7 @@
         <v>681</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>142</v>
@@ -20138,7 +20138,7 @@
         <v>231.2</v>
       </c>
       <c r="J231" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="K231" s="1">
         <v>352039</v>
@@ -20166,7 +20166,7 @@
         <v>779</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>200</v>
@@ -20190,7 +20190,7 @@
         <v>307.2</v>
       </c>
       <c r="J232" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="K232" s="1">
         <v>6912</v>
@@ -20199,10 +20199,10 @@
         <v>6646</v>
       </c>
       <c r="M232" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="N232" s="6" t="s">
         <v>822</v>
-      </c>
-      <c r="N232" s="6" t="s">
-        <v>823</v>
       </c>
       <c r="O232" s="9"/>
       <c r="P232" s="9"/>
@@ -20234,7 +20234,7 @@
         <v>777</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>200</v>
@@ -20258,7 +20258,7 @@
         <v>292</v>
       </c>
       <c r="J233" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="K233" s="1">
         <v>6602431</v>
@@ -20267,7 +20267,7 @@
         <v>5034782</v>
       </c>
       <c r="M233" s="6" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="N233" s="1"/>
       <c r="O233" s="9">
@@ -20308,7 +20308,7 @@
     <row r="234" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="B234" s="5" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
@@ -20348,7 +20348,7 @@
     <row r="235" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="B235" s="5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
@@ -20412,7 +20412,7 @@
     <row r="236" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="B236" s="5" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
@@ -20476,7 +20476,7 @@
     <row r="237" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="B237" s="5" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
@@ -20540,7 +20540,7 @@
     <row r="238" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="B238" s="5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
@@ -20592,7 +20592,7 @@
     <row r="239" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="B239" s="5" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
@@ -20656,7 +20656,7 @@
     <row r="240" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="B240" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -20720,7 +20720,7 @@
     <row r="241" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="B241" s="5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -20784,7 +20784,7 @@
     <row r="242" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" s="5" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -20824,7 +20824,7 @@
     <row r="243" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="B243" s="5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -20864,7 +20864,7 @@
     <row r="244" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" s="5" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C244" s="1"/>
       <c r="D244" s="1"/>
@@ -20904,7 +20904,7 @@
     <row r="245" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" s="5" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C245" s="1"/>
       <c r="D245" s="1"/>
@@ -20944,7 +20944,7 @@
     <row r="246" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="B246" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C246" s="1"/>
       <c r="D246" s="1"/>
@@ -20992,7 +20992,7 @@
     <row r="247" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="B247" s="5" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
@@ -21056,7 +21056,7 @@
     <row r="248" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="B248" s="5" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -21120,7 +21120,7 @@
     <row r="249" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" s="5" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -21160,7 +21160,7 @@
     <row r="250" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="B250" s="5" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C250" s="1"/>
       <c r="D250" s="1"/>
@@ -21200,7 +21200,7 @@
     <row r="251" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="B251" s="5" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C251" s="1"/>
       <c r="D251" s="1"/>
@@ -21240,7 +21240,7 @@
     <row r="252" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C252" s="1"/>
       <c r="D252" s="1"/>
@@ -21304,7 +21304,7 @@
     <row r="253" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C253" s="1"/>
       <c r="D253" s="1"/>
@@ -21686,7 +21686,7 @@
     <hyperlink ref="N225" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
     <hyperlink ref="M226" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
     <hyperlink ref="N226" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="M227" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="M227" r:id="rId320" display="C01368, C00105" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
     <hyperlink ref="N227" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
     <hyperlink ref="M228" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
     <hyperlink ref="N228" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>

</xml_diff>